<commit_message>
with speed and firing rate correlation updated
</commit_message>
<xml_diff>
--- a/UniversalParams.xlsx
+++ b/UniversalParams.xlsx
@@ -62,20 +62,28 @@
     <t>CellFileName</t>
   </si>
   <si>
-    <t>Cells_ContrastExperiment.xlsx</t>
-  </si>
-  <si>
-    <t>Y:\giocomo\export\data\Projects\ContrastExperiment_neuropixels\</t>
+    <t>UniversalParams.xlsx</t>
+  </si>
+  <si>
+    <t>\\oak-smb-giocomo.stanford.edu\groups\giocomo\ysun\Neuropixels</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -98,13 +106,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -385,13 +396,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="65.7109375" customWidth="1"/>
+    <col min="1" max="1" width="63.42578125" customWidth="1"/>
     <col min="2" max="2" width="30.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
@@ -439,7 +450,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B2" t="s">

</xml_diff>